<commit_message>
Provisional version of Report 3
</commit_message>
<xml_diff>
--- a/Practica 3. RNM/resultados.xlsx
+++ b/Practica 3. RNM/resultados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Nextcloud\ETSINF\2019-20\APR\Practicas\Practica 3. RNM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7180C4F4-05AD-47B6-A65B-7C8216778208}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D4D3AF-8747-49C3-BEA5-0490A01C13DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27300" windowHeight="15960" xr2:uid="{83A6FD4C-9625-4391-B922-2D675A9753B7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
   <si>
     <t>PCA</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>40 neurons HL</t>
+  </si>
+  <si>
+    <t>50% (error)</t>
+  </si>
+  <si>
+    <t>80% (error)</t>
   </si>
 </sst>
 </file>
@@ -165,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -176,16 +182,19 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -723,6 +732,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4.2799999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.28E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.2499999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1549,6 +1564,12 @@
                 <c:pt idx="2">
                   <c:v>4.2799999999999998E-2</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.28E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.2499999999999998E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1652,7 +1673,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$F$10</c:f>
+              <c:f>Sheet1!$B$16:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1774,7 +1795,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$F$11</c:f>
+              <c:f>Sheet1!$B$17:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1893,7 +1914,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$F$12</c:f>
+              <c:f>Sheet1!$B$18:$F$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2012,7 +2033,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$F$13</c:f>
+              <c:f>Sheet1!$B$19:$F$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2024,6 +2045,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3.4000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9899999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2460,7 +2484,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$F$10</c:f>
+              <c:f>Sheet1!$B$16:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2573,7 +2597,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$F$11</c:f>
+              <c:f>Sheet1!$B$17:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2686,7 +2710,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$F$12</c:f>
+              <c:f>Sheet1!$B$18:$F$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2799,7 +2823,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$F$13</c:f>
+              <c:f>Sheet1!$B$19:$F$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2811,6 +2835,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3.4000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9899999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4653,10 +4680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9BC3CE-F261-4AB7-92E6-ECAE26A45225}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F25" sqref="A20:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4665,7 +4692,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4">
+      <c r="A1" s="8">
         <v>0.5</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -4677,25 +4704,25 @@
       <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5">
+      <c r="A2" s="8"/>
+      <c r="B2" s="4">
         <v>10</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>20</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>30</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>40</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2">
@@ -4715,7 +4742,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2">
@@ -4735,7 +4762,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2">
@@ -4755,7 +4782,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3">
@@ -4767,124 +4794,415 @@
       <c r="D6" s="2">
         <v>4.2799999999999998E-2</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="E6" s="6">
+        <v>5.28E-2</v>
+      </c>
+      <c r="F6" s="6">
+        <v>5.2499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="4">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4">
+        <v>20</v>
+      </c>
+      <c r="D8" s="4">
+        <v>30</v>
+      </c>
+      <c r="E8" s="4">
+        <v>40</v>
+      </c>
+      <c r="F8" s="4">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5">
-        <v>10</v>
-      </c>
-      <c r="C9" s="5">
-        <v>20</v>
-      </c>
-      <c r="D9" s="5">
-        <v>30</v>
-      </c>
-      <c r="E9" s="5">
-        <v>40</v>
-      </c>
-      <c r="F9" s="5">
-        <v>50</v>
+      <c r="A9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT((B3/100)*(1-(B3/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.0318%</v>
+      </c>
+      <c r="C9" s="2" t="str">
+        <f t="shared" ref="C9:F9" si="0">"±"&amp;TEXT(100*(1.96*SQRT((C3/100)*(1-(C3/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.0253%</v>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>±0.0229%</v>
+      </c>
+      <c r="E9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>±0.0220%</v>
+      </c>
+      <c r="F9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>±0.0222%</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.14330000000000001</v>
-      </c>
-      <c r="C10" s="2">
-        <v>9.9500000000000005E-2</v>
-      </c>
-      <c r="D10" s="2">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="E10" s="2">
-        <v>7.3499999999999996E-2</v>
-      </c>
-      <c r="F10" s="2">
-        <v>7.2800000000000004E-2</v>
+      <c r="A10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <f t="shared" ref="B10:F10" si="1">"±"&amp;TEXT(100*(1.96*SQRT((B4/100)*(1-(B4/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.0242%</v>
+      </c>
+      <c r="C10" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>±0.0196%</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>±0.0194%</v>
+      </c>
+      <c r="E10" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>±0.0190%</v>
+      </c>
+      <c r="F10" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>±0.0194%</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2">
-        <v>9.5299999999999996E-2</v>
-      </c>
-      <c r="C11" s="3">
-        <v>5.4199999999999998E-2</v>
-      </c>
-      <c r="D11" s="2">
-        <v>4.8300000000000003E-2</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="F11" s="2">
-        <v>4.99E-2</v>
+      <c r="A11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="str">
+        <f t="shared" ref="B11:F11" si="2">"±"&amp;TEXT(100*(1.96*SQRT((B5/100)*(1-(B5/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.0229%</v>
+      </c>
+      <c r="C11" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>±0.0177%</v>
+      </c>
+      <c r="D11" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>±0.0173%</v>
+      </c>
+      <c r="E11" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>±0.0174%</v>
+      </c>
+      <c r="F11" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>±0.0166%</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="str">
+        <f t="shared" ref="B12:F12" si="3">"±"&amp;TEXT(100*(1.96*SQRT((B6/100)*(1-(B6/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.0226%</v>
+      </c>
+      <c r="C12" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>±0.0173%</v>
+      </c>
+      <c r="D12" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>±0.0166%</v>
+      </c>
+      <c r="E12" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>±0.0184%</v>
+      </c>
+      <c r="F12" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>±0.0183%</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="4">
+        <v>10</v>
+      </c>
+      <c r="C15" s="4">
+        <v>20</v>
+      </c>
+      <c r="D15" s="4">
+        <v>30</v>
+      </c>
+      <c r="E15" s="4">
+        <v>40</v>
+      </c>
+      <c r="F15" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.14330000000000001</v>
+      </c>
+      <c r="C16" s="2">
+        <v>9.9500000000000005E-2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="E16" s="2">
+        <v>7.3499999999999996E-2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>7.2800000000000004E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="2">
+        <v>9.5299999999999996E-2</v>
+      </c>
+      <c r="C17" s="3">
+        <v>5.4199999999999998E-2</v>
+      </c>
+      <c r="D17" s="2">
+        <v>4.8300000000000003E-2</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="F17" s="2">
+        <v>4.99E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B18" s="2">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C18" s="2">
         <v>4.6300000000000001E-2</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D18" s="2">
         <v>3.73E-2</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E18" s="2">
         <v>4.3400000000000001E-2</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F18" s="2">
         <v>3.9800000000000002E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B19" s="3">
         <v>7.3300000000000004E-2</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C19" s="2">
         <v>4.0300000000000002E-2</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D19" s="2">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="E19" s="6">
+        <v>3.9899999999999998E-2</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="4">
+        <v>10</v>
+      </c>
+      <c r="C21" s="4">
+        <v>20</v>
+      </c>
+      <c r="D21" s="4">
+        <v>30</v>
+      </c>
+      <c r="E21" s="4">
+        <v>40</v>
+      </c>
+      <c r="F21" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT((B16/100)*(1-(B16/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.0303%</v>
+      </c>
+      <c r="C22" s="2" t="str">
+        <f t="shared" ref="C22:F22" si="4">"±"&amp;TEXT(100*(1.96*SQRT((C16/100)*(1-(C16/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.0252%</v>
+      </c>
+      <c r="D22" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>±0.0222%</v>
+      </c>
+      <c r="E22" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>±0.0217%</v>
+      </c>
+      <c r="F22" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>±0.0216%</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="2" t="str">
+        <f t="shared" ref="B23:F23" si="5">"±"&amp;TEXT(100*(1.96*SQRT((B17/100)*(1-(B17/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.0247%</v>
+      </c>
+      <c r="C23" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>±0.0186%</v>
+      </c>
+      <c r="D23" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>±0.0176%</v>
+      </c>
+      <c r="E23" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>±0.0179%</v>
+      </c>
+      <c r="F23" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>±0.0179%</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2" t="str">
+        <f t="shared" ref="B24:F24" si="6">"±"&amp;TEXT(100*(1.96*SQRT((B18/100)*(1-(B18/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.0222%</v>
+      </c>
+      <c r="C24" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>±0.0172%</v>
+      </c>
+      <c r="D24" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>±0.0155%</v>
+      </c>
+      <c r="E24" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>±0.0167%</v>
+      </c>
+      <c r="F24" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>±0.0160%</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="2" t="str">
+        <f t="shared" ref="B25:F25" si="7">"±"&amp;TEXT(100*(1.96*SQRT((B19/100)*(1-(B19/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.0217%</v>
+      </c>
+      <c r="C25" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>±0.0161%</v>
+      </c>
+      <c r="D25" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>±0.0148%</v>
+      </c>
+      <c r="E25" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>±0.0160%</v>
+      </c>
+      <c r="F25" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:F20"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="B3:F6 B10:F13">
+  <conditionalFormatting sqref="B16:F19 B3:F6">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:F12">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22:F25">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>